<commit_message>
Ajout d'une activité dans le journal de Paul
</commit_message>
<xml_diff>
--- a/Journée d'activité/Paul.xlsx
+++ b/Journée d'activité/Paul.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CFB1EE-B8B5-40C5-9438-4F59A19693EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,16 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Découverte de Git et Github</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +58,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +340,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="74.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43777</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Avancement des Tahce + Modification  du Workbench
</commit_message>
<xml_diff>
--- a/Journée d'activité/Paul.xlsx
+++ b/Journée d'activité/Paul.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2CE8AB-466E-48F7-9B57-0A9E6733434B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00526F31-4BB8-4FE8-B526-7BEAEF3CA82B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>DATE</t>
   </si>
@@ -43,10 +43,13 @@
     <t>2.Implémentation de la Base De Données sur Php My Admin</t>
   </si>
   <si>
-    <t>3. Mise en commun en fin d'heure pour voir les différentes tâches qui ont été réalisées durant la séance.</t>
+    <t xml:space="preserve">Tâche à réaliser :  </t>
   </si>
   <si>
-    <t xml:space="preserve">Tâche à réaliser :  </t>
+    <t>4. Mise en commun en fin d'heure pour voir les différentes tâches qui ont été réalisées durant la séance.</t>
+  </si>
+  <si>
+    <t>3. Création d'un utilisateur ayant tous les droits les privilèges sur la BDD +  connexion a la base de donnée en php.</t>
   </si>
 </sst>
 </file>
@@ -242,11 +245,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -256,46 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -581,7 +581,7 @@
   <dimension ref="A2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:H9"/>
+      <selection activeCell="C11" sqref="C11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,102 +594,102 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11">
+      <c r="B4" s="2">
         <v>43777</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="8"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="11">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2">
         <v>43791</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="17" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="17" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -698,221 +698,216 @@
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="7"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="7"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="10"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="7"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="12"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="7"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="13"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="12"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="8"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="10"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="13"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="7"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="12"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="10"/>
+      <c r="H33" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
+  <mergeCells count="32">
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C22:H23"/>
+    <mergeCell ref="C26:H27"/>
+    <mergeCell ref="C28:H29"/>
+    <mergeCell ref="C30:H31"/>
     <mergeCell ref="C32:H33"/>
     <mergeCell ref="C24:H25"/>
     <mergeCell ref="B4:B5"/>
@@ -925,11 +920,19 @@
     <mergeCell ref="C12:H13"/>
     <mergeCell ref="C14:H15"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C22:H23"/>
-    <mergeCell ref="C26:H27"/>
-    <mergeCell ref="C28:H29"/>
-    <mergeCell ref="C30:H31"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modification de la clé primaire !
</commit_message>
<xml_diff>
--- a/Journée d'activité/Paul.xlsx
+++ b/Journée d'activité/Paul.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00526F31-4BB8-4FE8-B526-7BEAEF3CA82B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC940827-0902-498C-AA8D-7BA033E311AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>DATE</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>3. Création d'un utilisateur ayant tous les droits les privilèges sur la BDD +  connexion a la base de donnée en php.</t>
+  </si>
+  <si>
+    <t>Modification de la BDD , de certaines clé primaire qui nous étais pas utiles .</t>
   </si>
 </sst>
 </file>
@@ -85,7 +88,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -237,53 +240,57 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -295,7 +302,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -580,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:H11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,318 +628,324 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>43777</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="12"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="13"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="13"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3">
         <v>43791</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="8" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="3" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="12"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="13"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="12"/>
+      <c r="B14" s="3">
+        <v>43798</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="13"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="12"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="13"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="12"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="13"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="12"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="13"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="12"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="13"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="12"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="13"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="12"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="13"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="12"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="11"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="12"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="11"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="13"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="14"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="12"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="13"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C22:H23"/>
-    <mergeCell ref="C26:H27"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="C28:H29"/>
     <mergeCell ref="C30:H31"/>
     <mergeCell ref="C32:H33"/>
@@ -922,13 +962,11 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C22:H23"/>
+    <mergeCell ref="C26:H27"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="C10:H10"/>

</xml_diff>